<commit_message>
build process for exe
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,11 @@
           <t>name</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>color</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -455,6 +460,11 @@
           <t>p1</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>#e0f7fa</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -465,6 +475,11 @@
           <t>p2</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>#e0f7fa</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -475,6 +490,11 @@
           <t>sdsd</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>#e0f7fa</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -483,6 +503,11 @@
       <c r="B5" t="inlineStr">
         <is>
           <t>sdsf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>#e0f7fa</t>
         </is>
       </c>
     </row>
@@ -584,7 +609,11 @@
           <t>ongoing</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;sdkj&lt;/p&gt;&lt;p&gt;alsk&lt;/p&gt;&lt;ol&gt;&lt;li&gt;sd &lt;/li&gt;&lt;li&gt;&lt;br&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+        </is>
+      </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>

</xml_diff>